<commit_message>
array && array 2d implement && sample test
</commit_message>
<xml_diff>
--- a/tests/template-excel/sample-array-output.xlsx
+++ b/tests/template-excel/sample-array-output.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
   <si>
     <t>a1</t>
   </si>
@@ -29,7 +29,7 @@
     <t>d1</t>
   </si>
   <si>
-    <t>g1</t>
+    <t>i1</t>
   </si>
   <si>
     <t>a2</t>
@@ -38,7 +38,7 @@
     <t>b2</t>
   </si>
   <si>
-    <t>g2</t>
+    <t>i2</t>
   </si>
   <si>
     <t>some things</t>
@@ -53,7 +53,10 @@
     <t>e2</t>
   </si>
   <si>
-    <t>g3</t>
+    <t>x var</t>
+  </si>
+  <si>
+    <t>{i3}</t>
   </si>
   <si>
     <t>a4</t>
@@ -62,7 +65,25 @@
     <t>b4</t>
   </si>
   <si>
-    <t>I am origin g4</t>
+    <t>[A1]</t>
+  </si>
+  <si>
+    <t>move to i5</t>
+  </si>
+  <si>
+    <t>a9</t>
+  </si>
+  <si>
+    <t>a10</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>xx</t>
+  </si>
+  <si>
+    <t>{a11}</t>
   </si>
 </sst>
 </file>
@@ -398,10 +419,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -411,7 +432,7 @@
     <col min="9" max="9" width="14.75" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -431,8 +452,9 @@
       <c r="I1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1"/>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -445,8 +467,9 @@
       <c r="I2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2"/>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -462,25 +485,31 @@
       </c>
       <c r="F3"/>
       <c r="G3"/>
-      <c r="H3"/>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
       <c r="I3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>13</v>
+      </c>
+      <c r="J3"/>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4"/>
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
       <c r="F4"/>
       <c r="G4"/>
       <c r="H4"/>
       <c r="I4"/>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4"/>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5"/>
       <c r="B5"/>
       <c r="C5"/>
@@ -488,8 +517,85 @@
       <c r="G5"/>
       <c r="H5"/>
       <c r="I5" t="s">
-        <v>15</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="J5"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6"/>
+      <c r="B6"/>
+      <c r="C6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6"/>
+      <c r="J6"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7"/>
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8"/>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11"/>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11"/>
+      <c r="J11"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12"/>
+      <c r="C12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>